<commit_message>
add sth for this week's work
Signed-off-by: 夏廷东 <Eric@xiatingdongdeMacBook-Pro.local>
</commit_message>
<xml_diff>
--- a/0731-0806.xlsx
+++ b/0731-0806.xlsx
@@ -1,19 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Eric/Desktop/PERSONAL/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="700" yWindow="460" windowWidth="24900" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="每天进度" sheetId="1" r:id="rId1"/>
     <sheet name="整体计划" sheetId="2" r:id="rId2"/>
     <sheet name="目前跟进项目进度" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="78">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -319,11 +330,145 @@
 6 5:00-6:30.项目整理</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>2未完成</t>
+    <rPh sb="1" eb="2">
+      <t>wei wan cheng</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5未完成</t>
+    <rPh sb="1" eb="2">
+      <t>wei wan cheng</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基本合理</t>
+    <rPh sb="0" eb="1">
+      <t>ji ben he li</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1:项目整理2:建立沟通机制</t>
+    <rPh sb="2" eb="3">
+      <t>xiang mu</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>zheng li</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>jian li</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>gou tong ji zhi</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1:en
+2:职场运营法则
+3:项目规则</t>
+    <rPh sb="7" eb="8">
+      <t>zhi chang</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>yun ying fa ze</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>xiang mu</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>gui ze</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基本ok</t>
+    <rPh sb="0" eb="1">
+      <t>ji ben</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开车不发脾气</t>
+    <rPh sb="0" eb="1">
+      <t>kai che</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>bu fa pi qi</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晚上健身房，</t>
+    <rPh sb="0" eb="1">
+      <t>wan shang</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>jian shen fang</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1:消防工程师学习纳入日程
+2:职场法则读完
+3:项目梳理进行评审，
+4:gerrit自己搭建并使用</t>
+    <rPh sb="2" eb="3">
+      <t>xiao fang gong cheng shi</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>xue xi</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>na ru</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>ri cheng</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>zhi chang</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>fa ze</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>du wan</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>xiang mu</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>shu li</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>jin xing</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>ping shen</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>zi ji</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>da jian</t>
+    </rPh>
+    <rPh sb="47" eb="48">
+      <t>bing</t>
+    </rPh>
+    <rPh sb="48" eb="49">
+      <t>shi yong</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -410,86 +555,86 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -557,30 +702,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -599,11 +720,35 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -887,85 +1032,85 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3:M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="100" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5" style="15" customWidth="1"/>
     <col min="2" max="2" width="44" style="2" customWidth="1"/>
     <col min="3" max="3" width="21.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="36.75" style="2" customWidth="1"/>
+    <col min="4" max="4" width="36.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="26" style="2" customWidth="1"/>
     <col min="6" max="7" width="38" style="2" customWidth="1"/>
-    <col min="8" max="8" width="29.375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="34.25" style="2" customWidth="1"/>
-    <col min="10" max="10" width="25.125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="33.25" style="2" customWidth="1"/>
+    <col min="8" max="8" width="29.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="34.1640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="25.1640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="33.1640625" style="2" customWidth="1"/>
     <col min="12" max="12" width="43.5" style="2" customWidth="1"/>
     <col min="13" max="13" width="32" style="2" customWidth="1"/>
     <col min="14" max="14" width="11.5" style="2" customWidth="1"/>
     <col min="15" max="15" width="9" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="9" style="2"/>
+    <col min="16" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="11"/>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="27" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="12"/>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="31" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="13"/>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="36" t="s">
         <v>12</v>
       </c>
       <c r="J1" s="14"/>
-      <c r="K1" s="28" t="s">
+      <c r="K1" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="M1" s="29" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="32"/>
-      <c r="B2" s="34"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="36"/>
+      <c r="D2" s="28"/>
       <c r="E2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="38"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="32"/>
       <c r="H2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="27"/>
+      <c r="I2" s="37"/>
       <c r="J2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="23"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="33"/>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" ht="258.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
@@ -974,11 +1119,15 @@
       <c r="B3" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="16"/>
+      <c r="C3" s="16" t="s">
+        <v>70</v>
+      </c>
       <c r="D3" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
       <c r="H3" s="4"/>
@@ -986,8 +1135,10 @@
       <c r="J3" s="16"/>
       <c r="K3" s="16"/>
       <c r="L3" s="16"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="24"/>
+      <c r="M3" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="N3" s="34"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
@@ -996,20 +1147,34 @@
       <c r="B4" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="16"/>
+      <c r="C4" s="16" t="s">
+        <v>69</v>
+      </c>
       <c r="D4" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="16"/>
+      <c r="E4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>75</v>
+      </c>
       <c r="J4" s="5"/>
-      <c r="K4" s="17"/>
+      <c r="K4" s="17" t="s">
+        <v>76</v>
+      </c>
       <c r="L4" s="16"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="25"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="35"/>
     </row>
     <row r="5" spans="1:14" s="1" customFormat="1" ht="141" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
@@ -1026,7 +1191,7 @@
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
       <c r="L5" s="16"/>
-      <c r="M5" s="24"/>
+      <c r="M5" s="34"/>
     </row>
     <row r="6" spans="1:14" s="1" customFormat="1" ht="155.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
@@ -1043,7 +1208,7 @@
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
       <c r="L6" s="16"/>
-      <c r="M6" s="24"/>
+      <c r="M6" s="34"/>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" ht="219.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
@@ -1060,9 +1225,9 @@
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
       <c r="L7" s="16"/>
-      <c r="M7" s="24"/>
-    </row>
-    <row r="8" spans="1:14" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M7" s="34"/>
+    </row>
+    <row r="8" spans="1:14" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>42952</v>
       </c>
@@ -1077,9 +1242,9 @@
       <c r="J8" s="16"/>
       <c r="K8" s="16"/>
       <c r="L8" s="16"/>
-      <c r="M8" s="24"/>
-    </row>
-    <row r="9" spans="1:14" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M8" s="34"/>
+    </row>
+    <row r="9" spans="1:14" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>42953</v>
       </c>
@@ -1094,7 +1259,7 @@
       <c r="J9" s="16"/>
       <c r="K9" s="16"/>
       <c r="L9" s="16"/>
-      <c r="M9" s="25"/>
+      <c r="M9" s="35"/>
     </row>
     <row r="10" spans="1:14" s="1" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
@@ -1109,7 +1274,7 @@
       <c r="J10" s="16"/>
       <c r="K10" s="16"/>
       <c r="L10" s="16"/>
-      <c r="M10" s="23"/>
+      <c r="M10" s="33"/>
     </row>
     <row r="11" spans="1:14" s="1" customFormat="1" ht="171.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
@@ -1124,7 +1289,7 @@
       <c r="J11" s="16"/>
       <c r="K11" s="16"/>
       <c r="L11" s="16"/>
-      <c r="M11" s="24"/>
+      <c r="M11" s="34"/>
     </row>
     <row r="12" spans="1:14" s="1" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
@@ -1139,9 +1304,9 @@
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
       <c r="L12" s="16"/>
-      <c r="M12" s="24"/>
-    </row>
-    <row r="13" spans="1:14" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M12" s="34"/>
+    </row>
+    <row r="13" spans="1:14" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -1154,7 +1319,7 @@
       <c r="J13" s="16"/>
       <c r="K13" s="16"/>
       <c r="L13" s="16"/>
-      <c r="M13" s="24"/>
+      <c r="M13" s="34"/>
     </row>
     <row r="14" spans="1:14" s="1" customFormat="1" ht="129.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
@@ -1169,9 +1334,9 @@
       <c r="J14" s="16"/>
       <c r="K14" s="16"/>
       <c r="L14" s="16"/>
-      <c r="M14" s="25"/>
-    </row>
-    <row r="15" spans="1:14" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M14" s="35"/>
+    </row>
+    <row r="15" spans="1:14" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -1186,7 +1351,7 @@
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
     </row>
-    <row r="16" spans="1:14" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -1214,7 +1379,7 @@
       <c r="J17" s="16"/>
       <c r="K17" s="16"/>
       <c r="L17" s="16"/>
-      <c r="M17" s="23"/>
+      <c r="M17" s="33"/>
     </row>
     <row r="18" spans="1:13" s="1" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
@@ -1229,9 +1394,9 @@
       <c r="J18" s="16"/>
       <c r="K18" s="16"/>
       <c r="L18" s="16"/>
-      <c r="M18" s="24"/>
-    </row>
-    <row r="19" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M18" s="34"/>
+    </row>
+    <row r="19" spans="1:13" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -1244,7 +1409,7 @@
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
       <c r="L19" s="16"/>
-      <c r="M19" s="24"/>
+      <c r="M19" s="34"/>
     </row>
     <row r="20" spans="1:13" s="1" customFormat="1" ht="174.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
@@ -1259,9 +1424,9 @@
       <c r="J20" s="16"/>
       <c r="K20" s="16"/>
       <c r="L20" s="16"/>
-      <c r="M20" s="24"/>
-    </row>
-    <row r="21" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M20" s="34"/>
+    </row>
+    <row r="21" spans="1:13" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -1274,9 +1439,9 @@
       <c r="J21" s="16"/>
       <c r="K21" s="16"/>
       <c r="L21" s="16"/>
-      <c r="M21" s="24"/>
-    </row>
-    <row r="22" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M21" s="34"/>
+    </row>
+    <row r="22" spans="1:13" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
@@ -1289,9 +1454,9 @@
       <c r="J22" s="16"/>
       <c r="K22" s="16"/>
       <c r="L22" s="16"/>
-      <c r="M22" s="24"/>
-    </row>
-    <row r="23" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M22" s="34"/>
+    </row>
+    <row r="23" spans="1:13" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -1304,9 +1469,9 @@
       <c r="J23" s="16"/>
       <c r="K23" s="16"/>
       <c r="L23" s="16"/>
-      <c r="M23" s="25"/>
-    </row>
-    <row r="24" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M23" s="35"/>
+    </row>
+    <row r="24" spans="1:13" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
@@ -1321,7 +1486,7 @@
       <c r="L24" s="16"/>
       <c r="M24" s="16"/>
     </row>
-    <row r="25" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
@@ -1336,7 +1501,7 @@
       <c r="L25" s="16"/>
       <c r="M25" s="16"/>
     </row>
-    <row r="26" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -1351,7 +1516,7 @@
       <c r="L26" s="16"/>
       <c r="M26" s="16"/>
     </row>
-    <row r="27" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -1366,7 +1531,7 @@
       <c r="L27" s="16"/>
       <c r="M27" s="16"/>
     </row>
-    <row r="28" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -1381,7 +1546,7 @@
       <c r="L28" s="16"/>
       <c r="M28" s="16"/>
     </row>
-    <row r="29" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
@@ -1396,7 +1561,7 @@
       <c r="L29" s="16"/>
       <c r="M29" s="16"/>
     </row>
-    <row r="30" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="7"/>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
@@ -1411,7 +1576,7 @@
       <c r="L30" s="16"/>
       <c r="M30" s="16"/>
     </row>
-    <row r="31" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -1426,7 +1591,7 @@
       <c r="L31" s="16"/>
       <c r="M31" s="16"/>
     </row>
-    <row r="32" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -1443,11 +1608,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
     <mergeCell ref="M17:M23"/>
     <mergeCell ref="N2:N4"/>
     <mergeCell ref="I1:I2"/>
@@ -1456,6 +1616,11 @@
     <mergeCell ref="M3:M9"/>
     <mergeCell ref="M10:M14"/>
     <mergeCell ref="M1:M2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1471,14 +1636,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>15</v>
       </c>
@@ -1489,7 +1654,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1497,7 +1662,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1505,7 +1670,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1513,7 +1678,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="22">
         <v>4</v>
       </c>
@@ -1521,13 +1686,13 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>1</v>
       </c>
@@ -1535,7 +1700,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -1543,7 +1708,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>3</v>
       </c>
@@ -1551,7 +1716,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>4</v>
       </c>
@@ -1559,7 +1724,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>5</v>
       </c>
@@ -1567,13 +1732,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>1</v>
       </c>
@@ -1581,7 +1746,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>2</v>
       </c>
@@ -1589,13 +1754,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>1</v>
       </c>
@@ -1603,7 +1768,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>2</v>
       </c>
@@ -1626,17 +1791,17 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.875" customWidth="1"/>
-    <col min="2" max="2" width="9.375" customWidth="1"/>
-    <col min="3" max="3" width="20.625" customWidth="1"/>
-    <col min="4" max="4" width="26.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="12.125" customWidth="1"/>
-    <col min="8" max="8" width="12.875" customWidth="1"/>
-    <col min="9" max="9" width="30.125" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1668,7 +1833,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -1693,7 +1858,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
@@ -1710,7 +1875,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>39</v>
       </c>
@@ -1781,7 +1946,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1792,7 +1957,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1803,7 +1968,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1814,7 +1979,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1825,7 +1990,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1836,7 +2001,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1847,7 +2012,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1858,7 +2023,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1869,7 +2034,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1880,7 +2045,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1891,7 +2056,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1902,7 +2067,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1913,7 +2078,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1924,7 +2089,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1935,7 +2100,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1946,7 +2111,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1957,7 +2122,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1968,7 +2133,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1979,7 +2144,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1990,7 +2155,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2001,7 +2166,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2012,7 +2177,7 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2023,7 +2188,7 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2034,7 +2199,7 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2045,7 +2210,7 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2056,7 +2221,7 @@
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -2067,7 +2232,7 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -2078,7 +2243,7 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -2089,7 +2254,7 @@
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -2100,7 +2265,7 @@
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -2111,7 +2276,7 @@
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -2122,7 +2287,7 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2133,7 +2298,7 @@
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2144,7 +2309,7 @@
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -2155,7 +2320,7 @@
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
     </row>
-    <row r="41" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2166,7 +2331,7 @@
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2177,7 +2342,7 @@
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2188,7 +2353,7 @@
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2199,7 +2364,7 @@
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2210,7 +2375,7 @@
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
     </row>
-    <row r="46" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2221,7 +2386,7 @@
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
     </row>
-    <row r="47" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2232,7 +2397,7 @@
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
     </row>
-    <row r="48" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2243,7 +2408,7 @@
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
     </row>
-    <row r="49" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -2254,7 +2419,7 @@
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
     </row>
-    <row r="50" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2265,7 +2430,7 @@
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
     </row>
-    <row r="51" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -2276,7 +2441,7 @@
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
     </row>
-    <row r="52" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -2287,7 +2452,7 @@
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
     </row>
-    <row r="53" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -2298,7 +2463,7 @@
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
     </row>
-    <row r="54" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2309,7 +2474,7 @@
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
     </row>
-    <row r="55" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -2320,7 +2485,7 @@
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
     </row>
-    <row r="56" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -2331,7 +2496,7 @@
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
     </row>
-    <row r="57" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -2342,7 +2507,7 @@
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
     </row>
-    <row r="58" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -2353,7 +2518,7 @@
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
     </row>
-    <row r="59" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2364,7 +2529,7 @@
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
     </row>
-    <row r="60" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2375,7 +2540,7 @@
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
     </row>
-    <row r="61" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -2386,7 +2551,7 @@
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
     </row>
-    <row r="62" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2397,7 +2562,7 @@
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
     </row>
-    <row r="63" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2408,7 +2573,7 @@
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
     </row>
-    <row r="64" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2419,7 +2584,7 @@
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
     </row>
-    <row r="65" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2430,7 +2595,7 @@
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
     </row>
-    <row r="66" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2441,7 +2606,7 @@
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
     </row>
-    <row r="67" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2452,7 +2617,7 @@
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
     </row>
-    <row r="68" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2463,7 +2628,7 @@
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
     </row>
-    <row r="69" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2474,7 +2639,7 @@
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
     </row>
-    <row r="70" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2485,7 +2650,7 @@
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
     </row>
-    <row r="71" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2496,7 +2661,7 @@
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
     </row>
-    <row r="72" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2507,7 +2672,7 @@
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
     </row>
-    <row r="73" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2518,7 +2683,7 @@
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
     </row>
-    <row r="74" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2529,7 +2694,7 @@
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
     </row>
-    <row r="75" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2540,7 +2705,7 @@
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
     </row>
-    <row r="76" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2551,7 +2716,7 @@
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
     </row>
-    <row r="77" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2562,7 +2727,7 @@
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
     </row>
-    <row r="78" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2573,7 +2738,7 @@
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
     </row>
-    <row r="79" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2584,7 +2749,7 @@
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
     </row>
-    <row r="80" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2595,7 +2760,7 @@
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
     </row>
-    <row r="81" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2606,7 +2771,7 @@
       <c r="H81" s="2"/>
       <c r="I81" s="2"/>
     </row>
-    <row r="82" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2617,7 +2782,7 @@
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
     </row>
-    <row r="83" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2628,7 +2793,7 @@
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
     </row>
-    <row r="84" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2639,7 +2804,7 @@
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
     </row>
-    <row r="85" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2650,7 +2815,7 @@
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
     </row>
-    <row r="86" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2661,7 +2826,7 @@
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
     </row>
-    <row r="87" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2672,7 +2837,7 @@
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
     </row>
-    <row r="88" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2683,7 +2848,7 @@
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
     </row>
-    <row r="89" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2694,7 +2859,7 @@
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
     </row>
-    <row r="90" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2705,7 +2870,7 @@
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
     </row>
-    <row r="91" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2716,7 +2881,7 @@
       <c r="H91" s="2"/>
       <c r="I91" s="2"/>
     </row>
-    <row r="92" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -2727,7 +2892,7 @@
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
     </row>
-    <row r="93" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -2738,7 +2903,7 @@
       <c r="H93" s="2"/>
       <c r="I93" s="2"/>
     </row>
-    <row r="94" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -2749,7 +2914,7 @@
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
     </row>
-    <row r="95" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -2760,7 +2925,7 @@
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
     </row>
-    <row r="96" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2771,7 +2936,7 @@
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
     </row>
-    <row r="97" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2782,7 +2947,7 @@
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
     </row>
-    <row r="98" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -2793,7 +2958,7 @@
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
     </row>
-    <row r="99" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2804,7 +2969,7 @@
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
     </row>
-    <row r="100" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2815,7 +2980,7 @@
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
     </row>
-    <row r="101" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -2826,7 +2991,7 @@
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>
     </row>
-    <row r="102" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -2837,7 +3002,7 @@
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
     </row>
-    <row r="103" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -2848,7 +3013,7 @@
       <c r="H103" s="2"/>
       <c r="I103" s="2"/>
     </row>
-    <row r="104" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -2859,7 +3024,7 @@
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
     </row>
-    <row r="105" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -2870,7 +3035,7 @@
       <c r="H105" s="2"/>
       <c r="I105" s="2"/>
     </row>
-    <row r="106" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -2881,7 +3046,7 @@
       <c r="H106" s="2"/>
       <c r="I106" s="2"/>
     </row>
-    <row r="107" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -2892,7 +3057,7 @@
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
     </row>
-    <row r="108" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -2903,7 +3068,7 @@
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
     </row>
-    <row r="109" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -2914,7 +3079,7 @@
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
     </row>
-    <row r="110" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -2925,7 +3090,7 @@
       <c r="H110" s="2"/>
       <c r="I110" s="2"/>
     </row>
-    <row r="111" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -2936,7 +3101,7 @@
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
     </row>
-    <row r="112" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -2947,7 +3112,7 @@
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
     </row>
-    <row r="113" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -2958,7 +3123,7 @@
       <c r="H113" s="2"/>
       <c r="I113" s="2"/>
     </row>
-    <row r="114" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -2969,7 +3134,7 @@
       <c r="H114" s="2"/>
       <c r="I114" s="2"/>
     </row>
-    <row r="115" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -2980,7 +3145,7 @@
       <c r="H115" s="2"/>
       <c r="I115" s="2"/>
     </row>
-    <row r="116" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -2991,7 +3156,7 @@
       <c r="H116" s="2"/>
       <c r="I116" s="2"/>
     </row>
-    <row r="117" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -3002,7 +3167,7 @@
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
     </row>
-    <row r="118" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -3013,7 +3178,7 @@
       <c r="H118" s="2"/>
       <c r="I118" s="2"/>
     </row>
-    <row r="119" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -3024,7 +3189,7 @@
       <c r="H119" s="2"/>
       <c r="I119" s="2"/>
     </row>
-    <row r="120" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -3035,7 +3200,7 @@
       <c r="H120" s="2"/>
       <c r="I120" s="2"/>
     </row>
-    <row r="121" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -3046,7 +3211,7 @@
       <c r="H121" s="2"/>
       <c r="I121" s="2"/>
     </row>
-    <row r="122" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -3057,7 +3222,7 @@
       <c r="H122" s="2"/>
       <c r="I122" s="2"/>
     </row>
-    <row r="123" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -3068,7 +3233,7 @@
       <c r="H123" s="2"/>
       <c r="I123" s="2"/>
     </row>
-    <row r="124" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -3079,7 +3244,7 @@
       <c r="H124" s="2"/>
       <c r="I124" s="2"/>
     </row>
-    <row r="125" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -3090,7 +3255,7 @@
       <c r="H125" s="2"/>
       <c r="I125" s="2"/>
     </row>
-    <row r="126" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -3101,7 +3266,7 @@
       <c r="H126" s="2"/>
       <c r="I126" s="2"/>
     </row>
-    <row r="127" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -3112,7 +3277,7 @@
       <c r="H127" s="2"/>
       <c r="I127" s="2"/>
     </row>
-    <row r="128" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -3123,7 +3288,7 @@
       <c r="H128" s="2"/>
       <c r="I128" s="2"/>
     </row>
-    <row r="129" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -3134,7 +3299,7 @@
       <c r="H129" s="2"/>
       <c r="I129" s="2"/>
     </row>
-    <row r="130" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -3145,7 +3310,7 @@
       <c r="H130" s="2"/>
       <c r="I130" s="2"/>
     </row>
-    <row r="131" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -3156,7 +3321,7 @@
       <c r="H131" s="2"/>
       <c r="I131" s="2"/>
     </row>
-    <row r="132" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -3167,7 +3332,7 @@
       <c r="H132" s="2"/>
       <c r="I132" s="2"/>
     </row>
-    <row r="133" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -3178,7 +3343,7 @@
       <c r="H133" s="2"/>
       <c r="I133" s="2"/>
     </row>
-    <row r="134" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -3189,7 +3354,7 @@
       <c r="H134" s="2"/>
       <c r="I134" s="2"/>
     </row>
-    <row r="135" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -3200,7 +3365,7 @@
       <c r="H135" s="2"/>
       <c r="I135" s="2"/>
     </row>
-    <row r="136" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -3211,7 +3376,7 @@
       <c r="H136" s="2"/>
       <c r="I136" s="2"/>
     </row>
-    <row r="137" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -3222,7 +3387,7 @@
       <c r="H137" s="2"/>
       <c r="I137" s="2"/>
     </row>
-    <row r="138" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -3233,7 +3398,7 @@
       <c r="H138" s="2"/>
       <c r="I138" s="2"/>
     </row>
-    <row r="139" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -3244,7 +3409,7 @@
       <c r="H139" s="2"/>
       <c r="I139" s="2"/>
     </row>
-    <row r="140" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>

</xml_diff>

<commit_message>
add sth for 0802
Signed-off-by: user2 <xtd412@qq.com>
</commit_message>
<xml_diff>
--- a/0731-0806.xlsx
+++ b/0731-0806.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Eric/Desktop/PERSONAL/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="700" yWindow="460" windowWidth="24900" windowHeight="15540"/>
+    <workbookView xWindow="705" yWindow="465" windowWidth="24900" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="每天进度" sheetId="1" r:id="rId1"/>
@@ -21,18 +16,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="86">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -413,10 +408,55 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>1：9:00-10:00.GERRIT讨论会
+2：:110:30-1:50，oppo吃饭
+3:2:00-3:00，部门内部会议
+4：3:00-4:30.聚传拓展
+5:4:40-5:20.reading book
+6:5:30-6:30.项目整理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1:GERRIT讨论会
+2：项目梳理
+3：职场书籍
+4：聚传拓展</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基本合理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1：项目整理
+2：据传拓展
+3：GERRIT搭建</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1：en
+2：职场运营法则
+3：项目梳理流程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>练腹肌（玩一下动感单车）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>健身房</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>1:消防工程师学习纳入日程
 2:职场法则读完
 3:项目梳理进行评审，
-4:gerrit自己搭建并使用</t>
+4:gerrit自己搭建并使用
+:</t>
     <rPh sb="2" eb="3">
       <t>xiao fang gong cheng shi</t>
     </rPh>
@@ -468,7 +508,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1032,27 +1072,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:M9"/>
+    <sheetView tabSelected="1" topLeftCell="G3" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="100" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5" style="15" customWidth="1"/>
     <col min="2" max="2" width="44" style="2" customWidth="1"/>
     <col min="3" max="3" width="21.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="36.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="36.625" style="2" customWidth="1"/>
     <col min="5" max="5" width="26" style="2" customWidth="1"/>
     <col min="6" max="7" width="38" style="2" customWidth="1"/>
-    <col min="8" max="8" width="29.33203125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="34.1640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="25.1640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="33.1640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="29.375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="34.125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="25.125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="33.125" style="2" customWidth="1"/>
     <col min="12" max="12" width="43.5" style="2" customWidth="1"/>
     <col min="13" max="13" width="32" style="2" customWidth="1"/>
     <col min="14" max="14" width="11.5" style="2" customWidth="1"/>
     <col min="15" max="15" width="9" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="8.83203125" style="2"/>
+    <col min="16" max="16384" width="8.875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1136,11 +1176,11 @@
       <c r="K3" s="16"/>
       <c r="L3" s="16"/>
       <c r="M3" s="33" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="N3" s="34"/>
     </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" s="1" customFormat="1" ht="178.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>42948</v>
       </c>
@@ -1176,20 +1216,36 @@
       <c r="M4" s="34"/>
       <c r="N4" s="35"/>
     </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" ht="141" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" s="1" customFormat="1" ht="243" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>42949</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
+      <c r="B5" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>82</v>
+      </c>
       <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
+      <c r="I5" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
+      <c r="K5" s="16" t="s">
+        <v>84</v>
+      </c>
       <c r="L5" s="16"/>
       <c r="M5" s="34"/>
     </row>
@@ -1227,7 +1283,7 @@
       <c r="L7" s="16"/>
       <c r="M7" s="34"/>
     </row>
-    <row r="8" spans="1:14" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>42952</v>
       </c>
@@ -1244,7 +1300,7 @@
       <c r="L8" s="16"/>
       <c r="M8" s="34"/>
     </row>
-    <row r="9" spans="1:14" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>42953</v>
       </c>
@@ -1306,7 +1362,7 @@
       <c r="L12" s="16"/>
       <c r="M12" s="34"/>
     </row>
-    <row r="13" spans="1:14" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -1336,7 +1392,7 @@
       <c r="L14" s="16"/>
       <c r="M14" s="35"/>
     </row>
-    <row r="15" spans="1:14" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -1351,7 +1407,7 @@
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
     </row>
-    <row r="16" spans="1:14" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -1396,7 +1452,7 @@
       <c r="L18" s="16"/>
       <c r="M18" s="34"/>
     </row>
-    <row r="19" spans="1:13" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -1426,7 +1482,7 @@
       <c r="L20" s="16"/>
       <c r="M20" s="34"/>
     </row>
-    <row r="21" spans="1:13" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -1441,7 +1497,7 @@
       <c r="L21" s="16"/>
       <c r="M21" s="34"/>
     </row>
-    <row r="22" spans="1:13" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
@@ -1456,7 +1512,7 @@
       <c r="L22" s="16"/>
       <c r="M22" s="34"/>
     </row>
-    <row r="23" spans="1:13" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -1471,7 +1527,7 @@
       <c r="L23" s="16"/>
       <c r="M23" s="35"/>
     </row>
-    <row r="24" spans="1:13" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
@@ -1486,7 +1542,7 @@
       <c r="L24" s="16"/>
       <c r="M24" s="16"/>
     </row>
-    <row r="25" spans="1:13" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
@@ -1501,7 +1557,7 @@
       <c r="L25" s="16"/>
       <c r="M25" s="16"/>
     </row>
-    <row r="26" spans="1:13" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -1516,7 +1572,7 @@
       <c r="L26" s="16"/>
       <c r="M26" s="16"/>
     </row>
-    <row r="27" spans="1:13" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -1531,7 +1587,7 @@
       <c r="L27" s="16"/>
       <c r="M27" s="16"/>
     </row>
-    <row r="28" spans="1:13" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -1546,7 +1602,7 @@
       <c r="L28" s="16"/>
       <c r="M28" s="16"/>
     </row>
-    <row r="29" spans="1:13" s="1" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
@@ -1561,7 +1617,7 @@
       <c r="L29" s="16"/>
       <c r="M29" s="16"/>
     </row>
-    <row r="30" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="7"/>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
@@ -1576,7 +1632,7 @@
       <c r="L30" s="16"/>
       <c r="M30" s="16"/>
     </row>
-    <row r="31" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -1591,7 +1647,7 @@
       <c r="L31" s="16"/>
       <c r="M31" s="16"/>
     </row>
-    <row r="32" spans="1:13" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -1636,14 +1692,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>15</v>
       </c>
@@ -1654,7 +1710,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1662,7 +1718,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1670,7 +1726,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1678,7 +1734,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="22">
         <v>4</v>
       </c>
@@ -1686,13 +1742,13 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>1</v>
       </c>
@@ -1700,7 +1756,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -1708,7 +1764,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>3</v>
       </c>
@@ -1716,7 +1772,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>4</v>
       </c>
@@ -1724,7 +1780,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>5</v>
       </c>
@@ -1732,13 +1788,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>1</v>
       </c>
@@ -1746,7 +1802,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>2</v>
       </c>
@@ -1754,13 +1810,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>1</v>
       </c>
@@ -1768,7 +1824,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>2</v>
       </c>
@@ -1791,17 +1847,17 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.875" customWidth="1"/>
+    <col min="2" max="2" width="9.375" customWidth="1"/>
+    <col min="3" max="3" width="20.625" customWidth="1"/>
+    <col min="4" max="4" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" customWidth="1"/>
-    <col min="9" max="9" width="30.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12.125" customWidth="1"/>
+    <col min="8" max="8" width="12.875" customWidth="1"/>
+    <col min="9" max="9" width="30.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1833,7 +1889,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -1858,7 +1914,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
@@ -1875,7 +1931,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>39</v>
       </c>
@@ -1946,7 +2002,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1957,7 +2013,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1968,7 +2024,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1979,7 +2035,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1990,7 +2046,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2001,7 +2057,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2012,7 +2068,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2023,7 +2079,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2034,7 +2090,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2045,7 +2101,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2056,7 +2112,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2067,7 +2123,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2078,7 +2134,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2089,7 +2145,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2100,7 +2156,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2111,7 +2167,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -2122,7 +2178,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2133,7 +2189,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2144,7 +2200,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2155,7 +2211,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2166,7 +2222,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2177,7 +2233,7 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2188,7 +2244,7 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2199,7 +2255,7 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2210,7 +2266,7 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2221,7 +2277,7 @@
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -2232,7 +2288,7 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -2243,7 +2299,7 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -2254,7 +2310,7 @@
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -2265,7 +2321,7 @@
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -2276,7 +2332,7 @@
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -2287,7 +2343,7 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2298,7 +2354,7 @@
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2309,7 +2365,7 @@
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -2320,7 +2376,7 @@
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
     </row>
-    <row r="41" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2331,7 +2387,7 @@
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2342,7 +2398,7 @@
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2353,7 +2409,7 @@
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2364,7 +2420,7 @@
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2375,7 +2431,7 @@
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
     </row>
-    <row r="46" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2386,7 +2442,7 @@
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
     </row>
-    <row r="47" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2397,7 +2453,7 @@
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
     </row>
-    <row r="48" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2408,7 +2464,7 @@
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
     </row>
-    <row r="49" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -2419,7 +2475,7 @@
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
     </row>
-    <row r="50" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2430,7 +2486,7 @@
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
     </row>
-    <row r="51" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -2441,7 +2497,7 @@
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
     </row>
-    <row r="52" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -2452,7 +2508,7 @@
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
     </row>
-    <row r="53" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -2463,7 +2519,7 @@
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
     </row>
-    <row r="54" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2474,7 +2530,7 @@
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
     </row>
-    <row r="55" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -2485,7 +2541,7 @@
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
     </row>
-    <row r="56" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -2496,7 +2552,7 @@
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
     </row>
-    <row r="57" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -2507,7 +2563,7 @@
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
     </row>
-    <row r="58" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -2518,7 +2574,7 @@
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
     </row>
-    <row r="59" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2529,7 +2585,7 @@
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
     </row>
-    <row r="60" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2540,7 +2596,7 @@
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
     </row>
-    <row r="61" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -2551,7 +2607,7 @@
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
     </row>
-    <row r="62" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2562,7 +2618,7 @@
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
     </row>
-    <row r="63" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2573,7 +2629,7 @@
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
     </row>
-    <row r="64" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2584,7 +2640,7 @@
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
     </row>
-    <row r="65" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2595,7 +2651,7 @@
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
     </row>
-    <row r="66" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2606,7 +2662,7 @@
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
     </row>
-    <row r="67" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2617,7 +2673,7 @@
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
     </row>
-    <row r="68" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2628,7 +2684,7 @@
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
     </row>
-    <row r="69" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2639,7 +2695,7 @@
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
     </row>
-    <row r="70" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2650,7 +2706,7 @@
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
     </row>
-    <row r="71" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2661,7 +2717,7 @@
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
     </row>
-    <row r="72" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2672,7 +2728,7 @@
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
     </row>
-    <row r="73" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2683,7 +2739,7 @@
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
     </row>
-    <row r="74" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2694,7 +2750,7 @@
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
     </row>
-    <row r="75" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2705,7 +2761,7 @@
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
     </row>
-    <row r="76" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2716,7 +2772,7 @@
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
     </row>
-    <row r="77" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2727,7 +2783,7 @@
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
     </row>
-    <row r="78" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2738,7 +2794,7 @@
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
     </row>
-    <row r="79" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2749,7 +2805,7 @@
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
     </row>
-    <row r="80" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2760,7 +2816,7 @@
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
     </row>
-    <row r="81" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2771,7 +2827,7 @@
       <c r="H81" s="2"/>
       <c r="I81" s="2"/>
     </row>
-    <row r="82" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2782,7 +2838,7 @@
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
     </row>
-    <row r="83" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2793,7 +2849,7 @@
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
     </row>
-    <row r="84" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2804,7 +2860,7 @@
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
     </row>
-    <row r="85" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2815,7 +2871,7 @@
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
     </row>
-    <row r="86" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2826,7 +2882,7 @@
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
     </row>
-    <row r="87" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2837,7 +2893,7 @@
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
     </row>
-    <row r="88" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -2848,7 +2904,7 @@
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
     </row>
-    <row r="89" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2859,7 +2915,7 @@
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
     </row>
-    <row r="90" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2870,7 +2926,7 @@
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
     </row>
-    <row r="91" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2881,7 +2937,7 @@
       <c r="H91" s="2"/>
       <c r="I91" s="2"/>
     </row>
-    <row r="92" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -2892,7 +2948,7 @@
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
     </row>
-    <row r="93" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -2903,7 +2959,7 @@
       <c r="H93" s="2"/>
       <c r="I93" s="2"/>
     </row>
-    <row r="94" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -2914,7 +2970,7 @@
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
     </row>
-    <row r="95" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -2925,7 +2981,7 @@
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
     </row>
-    <row r="96" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -2936,7 +2992,7 @@
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
     </row>
-    <row r="97" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2947,7 +3003,7 @@
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
     </row>
-    <row r="98" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -2958,7 +3014,7 @@
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
     </row>
-    <row r="99" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2969,7 +3025,7 @@
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
     </row>
-    <row r="100" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2980,7 +3036,7 @@
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
     </row>
-    <row r="101" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -2991,7 +3047,7 @@
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>
     </row>
-    <row r="102" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -3002,7 +3058,7 @@
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
     </row>
-    <row r="103" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -3013,7 +3069,7 @@
       <c r="H103" s="2"/>
       <c r="I103" s="2"/>
     </row>
-    <row r="104" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -3024,7 +3080,7 @@
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
     </row>
-    <row r="105" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -3035,7 +3091,7 @@
       <c r="H105" s="2"/>
       <c r="I105" s="2"/>
     </row>
-    <row r="106" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -3046,7 +3102,7 @@
       <c r="H106" s="2"/>
       <c r="I106" s="2"/>
     </row>
-    <row r="107" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -3057,7 +3113,7 @@
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
     </row>
-    <row r="108" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -3068,7 +3124,7 @@
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
     </row>
-    <row r="109" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -3079,7 +3135,7 @@
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
     </row>
-    <row r="110" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -3090,7 +3146,7 @@
       <c r="H110" s="2"/>
       <c r="I110" s="2"/>
     </row>
-    <row r="111" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -3101,7 +3157,7 @@
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
     </row>
-    <row r="112" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -3112,7 +3168,7 @@
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
     </row>
-    <row r="113" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -3123,7 +3179,7 @@
       <c r="H113" s="2"/>
       <c r="I113" s="2"/>
     </row>
-    <row r="114" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -3134,7 +3190,7 @@
       <c r="H114" s="2"/>
       <c r="I114" s="2"/>
     </row>
-    <row r="115" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -3145,7 +3201,7 @@
       <c r="H115" s="2"/>
       <c r="I115" s="2"/>
     </row>
-    <row r="116" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -3156,7 +3212,7 @@
       <c r="H116" s="2"/>
       <c r="I116" s="2"/>
     </row>
-    <row r="117" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -3167,7 +3223,7 @@
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
     </row>
-    <row r="118" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -3178,7 +3234,7 @@
       <c r="H118" s="2"/>
       <c r="I118" s="2"/>
     </row>
-    <row r="119" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -3189,7 +3245,7 @@
       <c r="H119" s="2"/>
       <c r="I119" s="2"/>
     </row>
-    <row r="120" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -3200,7 +3256,7 @@
       <c r="H120" s="2"/>
       <c r="I120" s="2"/>
     </row>
-    <row r="121" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -3211,7 +3267,7 @@
       <c r="H121" s="2"/>
       <c r="I121" s="2"/>
     </row>
-    <row r="122" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -3222,7 +3278,7 @@
       <c r="H122" s="2"/>
       <c r="I122" s="2"/>
     </row>
-    <row r="123" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -3233,7 +3289,7 @@
       <c r="H123" s="2"/>
       <c r="I123" s="2"/>
     </row>
-    <row r="124" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -3244,7 +3300,7 @@
       <c r="H124" s="2"/>
       <c r="I124" s="2"/>
     </row>
-    <row r="125" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -3255,7 +3311,7 @@
       <c r="H125" s="2"/>
       <c r="I125" s="2"/>
     </row>
-    <row r="126" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -3266,7 +3322,7 @@
       <c r="H126" s="2"/>
       <c r="I126" s="2"/>
     </row>
-    <row r="127" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -3277,7 +3333,7 @@
       <c r="H127" s="2"/>
       <c r="I127" s="2"/>
     </row>
-    <row r="128" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -3288,7 +3344,7 @@
       <c r="H128" s="2"/>
       <c r="I128" s="2"/>
     </row>
-    <row r="129" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -3299,7 +3355,7 @@
       <c r="H129" s="2"/>
       <c r="I129" s="2"/>
     </row>
-    <row r="130" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -3310,7 +3366,7 @@
       <c r="H130" s="2"/>
       <c r="I130" s="2"/>
     </row>
-    <row r="131" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -3321,7 +3377,7 @@
       <c r="H131" s="2"/>
       <c r="I131" s="2"/>
     </row>
-    <row r="132" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -3332,7 +3388,7 @@
       <c r="H132" s="2"/>
       <c r="I132" s="2"/>
     </row>
-    <row r="133" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -3343,7 +3399,7 @@
       <c r="H133" s="2"/>
       <c r="I133" s="2"/>
     </row>
-    <row r="134" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -3354,7 +3410,7 @@
       <c r="H134" s="2"/>
       <c r="I134" s="2"/>
     </row>
-    <row r="135" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -3365,7 +3421,7 @@
       <c r="H135" s="2"/>
       <c r="I135" s="2"/>
     </row>
-    <row r="136" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -3376,7 +3432,7 @@
       <c r="H136" s="2"/>
       <c r="I136" s="2"/>
     </row>
-    <row r="137" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -3387,7 +3443,7 @@
       <c r="H137" s="2"/>
       <c r="I137" s="2"/>
     </row>
-    <row r="138" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -3398,7 +3454,7 @@
       <c r="H138" s="2"/>
       <c r="I138" s="2"/>
     </row>
-    <row r="139" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -3409,7 +3465,7 @@
       <c r="H139" s="2"/>
       <c r="I139" s="2"/>
     </row>
-    <row r="140" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>

</xml_diff>